<commit_message>
feat: The excel sheet for the tests has been completed along with the codes for the unit testing. fix: Some changes have been made to the client.py file in the name mangling so that tests are successfully running.
</commit_message>
<xml_diff>
--- a/tests/A01_pixell_test_plan_client.xlsx
+++ b/tests/A01_pixell_test_plan_client.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d1fc90ed9f3e2029/Desktop/RRC POLYTECH/Semester 2/intermediate_software_development/project/isd_project/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="13_ncr:1_{5ECD6C5C-0BF7-4659-811B-1D416A6C1BBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F513730-F220-4F75-816A-A7C14BC99BCB}"/>
+  <xr:revisionPtr revIDLastSave="72" documentId="13_ncr:1_{5ECD6C5C-0BF7-4659-811B-1D416A6C1BBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DDCC81BC-174D-4C4C-9B80-601C42A91B62}"/>
   <bookViews>
-    <workbookView xWindow="792" yWindow="1608" windowWidth="13272" windowHeight="8880" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -183,7 +183,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
   <si>
     <t>Software Development Team - Unit Test Plan</t>
   </si>
@@ -197,9 +197,6 @@
     <t>Client</t>
   </si>
   <si>
-    <t>Test Case ID</t>
-  </si>
-  <si>
     <t>Method Being Tested</t>
   </si>
   <si>
@@ -281,21 +278,12 @@
     <t>The attributes should be listed in a specific format.</t>
   </si>
   <si>
-    <t>Clinton, Anne [1212] - anne.clinton@pixellriver.com</t>
-  </si>
-  <si>
     <t>client_number = 1212 first_name = " " last_name = "Clinton" email_address = anne.clinton@pixellriver.com</t>
   </si>
   <si>
-    <t>client_number = abc first_name = "Anne" last_name = "Clinton" email_address = anne.clinton@pixellriver.com</t>
-  </si>
-  <si>
     <t>client_number = 1212 first_name = "Anne" last_name = " " email_address = anne.clinton@pixellriver.com</t>
   </si>
   <si>
-    <t>client_number = 1212 first_name = "Anne" last_name = " " email_address = anne.clinton.gmail.com</t>
-  </si>
-  <si>
     <t>Raises ValueError("The client number should be an integer.")</t>
   </si>
   <si>
@@ -306,13 +294,50 @@
   </si>
   <si>
     <t>Raises ValueError("The email_address is not valid.")</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>client_number=1212, first_name="Anne", last_name="Clinton", email_address="anne.clinton@pixellriver.com"</t>
+  </si>
+  <si>
+    <t>client_number = "abc" first_name = "Anne" last_name = "Clinton" email_address = anne.clinton@pixellriver.com</t>
+  </si>
+  <si>
+    <t>Returns 1212</t>
+  </si>
+  <si>
+    <t>Returns "Anne"</t>
+  </si>
+  <si>
+    <t>Returns "Clinton"</t>
+  </si>
+  <si>
+    <t>Returns "anne.clinton.pixelriver.com"</t>
+  </si>
+  <si>
+    <t>client_number = 1212 first_name = "Anne" last_name = "Clinton " email_address = "anne.clinton.pixelriver.com"</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Returns </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>"Clinton, Anne [1212] - anne.clinton@pixellriver.com"</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -373,6 +398,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -576,6 +606,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -599,9 +632,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -802,7 +832,7 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7B0B8C9F-A34D-46F3-9066-19FDAF76B033}" name="Table1" displayName="Table1" ref="B6:G28" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{B4BB882C-2019-4F87-8900-426FA9A11FFB}" name="Test Case ID" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{B4BB882C-2019-4F87-8900-426FA9A11FFB}" name="client_number=1212, first_name=&quot;Anne&quot;, last_name=&quot;Clinton&quot;, email_address=&quot;anne.clinton@pixellriver.com&quot;" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{1904C92F-9639-4229-AA4E-4C4DEAF21EEE}" name="Method Being Tested" dataDxfId="4"/>
     <tableColumn id="3" xr3:uid="{4E480EB6-99FB-4F51-98B5-D5BE13327E8C}" name="Condition Being Tested" dataDxfId="3"/>
     <tableColumn id="4" xr3:uid="{5381561B-09C5-439D-999E-CD8E013F9561}" name="Preconditions" dataDxfId="2"/>
@@ -1132,246 +1162,276 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DADEBCC4-BB44-48CD-B9AB-1E2FD3EE0EEB}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D10" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D6" zoomScale="106" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="2" width="12.6640625" customWidth="1"/>
     <col min="3" max="3" width="22.33203125" customWidth="1"/>
     <col min="4" max="4" width="32.6640625" customWidth="1"/>
     <col min="5" max="5" width="29.109375" customWidth="1"/>
-    <col min="6" max="6" width="35.44140625" customWidth="1"/>
-    <col min="7" max="7" width="44.33203125" customWidth="1"/>
+    <col min="6" max="6" width="36.6640625" customWidth="1"/>
+    <col min="7" max="7" width="60.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:7" ht="73.2" customHeight="1" thickBot="1" x14ac:dyDescent="1.8">
+    <row r="1" spans="1:7" ht="15" thickBot="1"/>
+    <row r="2" spans="1:7" ht="73.2" customHeight="1" thickBot="1">
       <c r="B2" s="2" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="14"/>
-    </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="15"/>
+    </row>
+    <row r="3" spans="1:7" ht="15" thickBot="1">
       <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="16"/>
-    </row>
-    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C3" s="16"/>
+      <c r="D3" s="17"/>
+    </row>
+    <row r="4" spans="1:7" ht="15" thickBot="1">
       <c r="B4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="18"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D4" s="19"/>
+    </row>
+    <row r="5" spans="1:7">
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="10" t="s">
+    <row r="6" spans="1:7">
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="D6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="E6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="F6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="G6" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:7" ht="76.2" customHeight="1">
       <c r="A7" s="4"/>
       <c r="B7" s="9">
         <v>1</v>
       </c>
       <c r="C7" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
+      <c r="E7" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>38</v>
+      </c>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="76.2" customHeight="1">
       <c r="A8" s="4"/>
       <c r="B8" s="11">
         <v>2</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="7"/>
+        <v>11</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>37</v>
+      </c>
       <c r="F8" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="G8" s="20" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="66" customHeight="1">
       <c r="A9" s="4"/>
       <c r="B9" s="11">
         <v>3</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="7"/>
+        <v>12</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>37</v>
+      </c>
       <c r="F9" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="66" customHeight="1">
       <c r="A10" s="4"/>
       <c r="B10" s="9">
         <v>4</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="7"/>
+        <v>13</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>37</v>
+      </c>
       <c r="F10" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G10" s="7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:7" ht="66" customHeight="1">
       <c r="A11" s="4"/>
       <c r="B11" s="11">
         <v>5</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="7"/>
+        <v>14</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>37</v>
+      </c>
       <c r="F11" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="G11" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:7" ht="31.2" customHeight="1">
       <c r="B12" s="11">
         <v>6</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="E12" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" s="20"/>
-      <c r="G12" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="31.2" customHeight="1">
       <c r="B13" s="9">
         <v>7</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="E13" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13" s="20"/>
-      <c r="G13" s="7"/>
-    </row>
-    <row r="14" spans="1:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="31.2" customHeight="1">
       <c r="B14" s="11">
         <v>8</v>
       </c>
       <c r="C14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="E14" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="F14" s="20"/>
-      <c r="G14" s="7"/>
-    </row>
-    <row r="15" spans="1:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="31.2" customHeight="1">
       <c r="B15" s="11">
         <v>9</v>
       </c>
       <c r="C15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="E15" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-    </row>
-    <row r="16" spans="1:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="31.2" customHeight="1">
       <c r="B16" s="9">
         <v>10</v>
       </c>
       <c r="C16" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="E16" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-    </row>
-    <row r="17" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="31.2" customHeight="1">
       <c r="B17" s="11">
         <v>11</v>
       </c>
@@ -1379,9 +1439,8 @@
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-    </row>
-    <row r="18" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="2:7" ht="31.2" customHeight="1">
       <c r="B18" s="11">
         <v>12</v>
       </c>
@@ -1391,7 +1450,7 @@
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:7" ht="31.2" customHeight="1">
       <c r="B19" s="9">
         <v>13</v>
       </c>
@@ -1401,7 +1460,7 @@
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:7" ht="31.2" customHeight="1">
       <c r="B20" s="11">
         <v>14</v>
       </c>
@@ -1411,7 +1470,7 @@
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:7" ht="31.2" customHeight="1">
       <c r="B21" s="11">
         <v>15</v>
       </c>
@@ -1421,7 +1480,7 @@
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:7" ht="31.2" customHeight="1">
       <c r="B22" s="9">
         <v>16</v>
       </c>
@@ -1431,7 +1490,7 @@
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:7" ht="31.2" customHeight="1">
       <c r="B23" s="11">
         <v>17</v>
       </c>
@@ -1441,7 +1500,7 @@
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:7" ht="31.2" customHeight="1">
       <c r="B24" s="11">
         <v>18</v>
       </c>
@@ -1451,7 +1510,7 @@
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:7" ht="31.2" customHeight="1">
       <c r="B25" s="9">
         <v>19</v>
       </c>
@@ -1461,7 +1520,7 @@
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:7" ht="31.2" customHeight="1">
       <c r="B26" s="11">
         <v>20</v>
       </c>
@@ -1471,7 +1530,7 @@
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
     </row>
-    <row r="27" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:7" ht="31.2" customHeight="1">
       <c r="B27" s="11">
         <v>21</v>
       </c>
@@ -1481,7 +1540,7 @@
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
     </row>
-    <row r="28" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:7" ht="31.2" customHeight="1">
       <c r="B28" s="9">
         <v>22</v>
       </c>
@@ -1491,15 +1550,15 @@
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B30" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
+    <row r="30" spans="2:7">
+      <c r="B30" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>